<commit_message>
Update results file with results from 03-29
* Added a tab that has average numbers by participant
</commit_message>
<xml_diff>
--- a/Phase 3 - Experiment/Results.xlsx
+++ b/Phase 3 - Experiment/Results.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="RawData" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="AvgByParticipant" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="21">
   <si>
     <t xml:space="preserve">Experiment Results</t>
   </si>
@@ -53,6 +54,36 @@
   </si>
   <si>
     <t xml:space="preserve">zooming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg scrolling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg zooming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average speed and accuracy by participant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Touchband</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scrolling time (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scrolling accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zooming time (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zooming accuracy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">zooming accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average</t>
   </si>
 </sst>
 </file>
@@ -177,10 +208,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -253,8 +284,12 @@
       <c r="D4" s="0" t="n">
         <v>13460</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">D4/1000</f>
+        <v>13.46</v>
+      </c>
       <c r="F4" s="0" t="n">
-        <v>1.666666666</v>
+        <v>0.1666666666</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>11</v>
@@ -265,6 +300,10 @@
       <c r="J4" s="0" t="n">
         <v>4696</v>
       </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">J4/1000</f>
+        <v>4.696</v>
+      </c>
       <c r="L4" s="0" t="n">
         <v>0.936883</v>
       </c>
@@ -279,6 +318,10 @@
       <c r="D5" s="0" t="n">
         <v>8306</v>
       </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">D5/1000</f>
+        <v>8.306</v>
+      </c>
       <c r="F5" s="0" t="n">
         <v>1</v>
       </c>
@@ -291,6 +334,10 @@
       <c r="J5" s="0" t="n">
         <v>5090</v>
       </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">J5/1000</f>
+        <v>5.09</v>
+      </c>
       <c r="L5" s="0" t="n">
         <v>0.928704</v>
       </c>
@@ -305,6 +352,10 @@
       <c r="D6" s="0" t="n">
         <v>4536</v>
       </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">D6/1000</f>
+        <v>4.536</v>
+      </c>
       <c r="F6" s="0" t="n">
         <v>1</v>
       </c>
@@ -317,6 +368,10 @@
       <c r="J6" s="0" t="n">
         <v>6043</v>
       </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">J6/1000</f>
+        <v>6.043</v>
+      </c>
       <c r="L6" s="0" t="n">
         <v>0.95679</v>
       </c>
@@ -331,6 +386,10 @@
       <c r="D7" s="0" t="n">
         <v>4291</v>
       </c>
+      <c r="E7" s="0" t="n">
+        <f aca="false">D7/1000</f>
+        <v>4.291</v>
+      </c>
       <c r="F7" s="0" t="n">
         <v>1</v>
       </c>
@@ -343,6 +402,10 @@
       <c r="J7" s="0" t="n">
         <v>5314</v>
       </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">J7/1000</f>
+        <v>5.314</v>
+      </c>
       <c r="L7" s="0" t="n">
         <v>0.764352</v>
       </c>
@@ -357,6 +420,10 @@
       <c r="D8" s="0" t="n">
         <v>5430</v>
       </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">D8/1000</f>
+        <v>5.43</v>
+      </c>
       <c r="F8" s="0" t="n">
         <v>1</v>
       </c>
@@ -369,6 +436,10 @@
       <c r="J8" s="0" t="n">
         <v>4300</v>
       </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">J8/1000</f>
+        <v>4.3</v>
+      </c>
       <c r="L8" s="0" t="n">
         <v>0.986883</v>
       </c>
@@ -383,6 +454,10 @@
       <c r="D9" s="0" t="n">
         <v>3672</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <f aca="false">D9/1000</f>
+        <v>3.672</v>
+      </c>
       <c r="F9" s="0" t="n">
         <v>1</v>
       </c>
@@ -395,6 +470,10 @@
       <c r="J9" s="0" t="n">
         <v>7041</v>
       </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">J9/1000</f>
+        <v>7.041</v>
+      </c>
       <c r="L9" s="0" t="n">
         <v>0.988889</v>
       </c>
@@ -409,6 +488,10 @@
       <c r="D10" s="0" t="n">
         <v>4266</v>
       </c>
+      <c r="E10" s="0" t="n">
+        <f aca="false">D10/1000</f>
+        <v>4.266</v>
+      </c>
       <c r="F10" s="0" t="n">
         <v>1</v>
       </c>
@@ -421,6 +504,10 @@
       <c r="J10" s="0" t="n">
         <v>5455</v>
       </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">J10/1000</f>
+        <v>5.455</v>
+      </c>
       <c r="L10" s="0" t="n">
         <v>0.800308</v>
       </c>
@@ -435,6 +522,10 @@
       <c r="D11" s="0" t="n">
         <v>6606</v>
       </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">D11/1000</f>
+        <v>6.606</v>
+      </c>
       <c r="F11" s="0" t="n">
         <v>1</v>
       </c>
@@ -447,6 +538,10 @@
       <c r="J11" s="0" t="n">
         <v>26367</v>
       </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">J11/1000</f>
+        <v>26.367</v>
+      </c>
       <c r="L11" s="0" t="n">
         <v>1</v>
       </c>
@@ -461,6 +556,10 @@
       <c r="D12" s="0" t="n">
         <v>6345</v>
       </c>
+      <c r="E12" s="0" t="n">
+        <f aca="false">D12/1000</f>
+        <v>6.345</v>
+      </c>
       <c r="F12" s="0" t="n">
         <v>1</v>
       </c>
@@ -473,6 +572,10 @@
       <c r="J12" s="0" t="n">
         <v>27766</v>
       </c>
+      <c r="K12" s="0" t="n">
+        <f aca="false">J12/1000</f>
+        <v>27.766</v>
+      </c>
       <c r="L12" s="0" t="n">
         <v>1</v>
       </c>
@@ -487,6 +590,10 @@
       <c r="D13" s="0" t="n">
         <v>4279</v>
       </c>
+      <c r="E13" s="0" t="n">
+        <f aca="false">D13/1000</f>
+        <v>4.279</v>
+      </c>
       <c r="F13" s="0" t="n">
         <v>1</v>
       </c>
@@ -499,6 +606,10 @@
       <c r="J13" s="0" t="n">
         <v>38954</v>
       </c>
+      <c r="K13" s="0" t="n">
+        <f aca="false">J13/1000</f>
+        <v>38.954</v>
+      </c>
       <c r="L13" s="0" t="n">
         <v>0.5</v>
       </c>
@@ -513,6 +624,10 @@
       <c r="D14" s="0" t="n">
         <v>6719</v>
       </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">D14/1000</f>
+        <v>6.719</v>
+      </c>
       <c r="F14" s="0" t="n">
         <v>0.662037</v>
       </c>
@@ -525,6 +640,10 @@
       <c r="J14" s="0" t="n">
         <v>41198</v>
       </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">J14/1000</f>
+        <v>41.198</v>
+      </c>
       <c r="L14" s="0" t="n">
         <v>1</v>
       </c>
@@ -539,6 +658,10 @@
       <c r="D15" s="0" t="n">
         <v>5670</v>
       </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">D15/1000</f>
+        <v>5.67</v>
+      </c>
       <c r="F15" s="0" t="n">
         <v>0.999074</v>
       </c>
@@ -551,6 +674,10 @@
       <c r="J15" s="0" t="n">
         <v>68394</v>
       </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">J15/1000</f>
+        <v>68.394</v>
+      </c>
       <c r="L15" s="0" t="n">
         <v>1</v>
       </c>
@@ -565,6 +692,10 @@
       <c r="D16" s="0" t="n">
         <v>4699</v>
       </c>
+      <c r="E16" s="0" t="n">
+        <f aca="false">D16/1000</f>
+        <v>4.699</v>
+      </c>
       <c r="F16" s="0" t="n">
         <v>0.928704</v>
       </c>
@@ -577,6 +708,10 @@
       <c r="J16" s="0" t="n">
         <v>301022</v>
       </c>
+      <c r="K16" s="0" t="n">
+        <f aca="false">J16/1000</f>
+        <v>301.022</v>
+      </c>
       <c r="L16" s="0" t="n">
         <v>0.5</v>
       </c>
@@ -591,6 +726,10 @@
       <c r="D17" s="0" t="n">
         <v>4401</v>
       </c>
+      <c r="E17" s="0" t="n">
+        <f aca="false">D17/1000</f>
+        <v>4.401</v>
+      </c>
       <c r="F17" s="0" t="n">
         <v>0.928704</v>
       </c>
@@ -603,6 +742,10 @@
       <c r="J17" s="0" t="n">
         <v>46759</v>
       </c>
+      <c r="K17" s="0" t="n">
+        <f aca="false">J17/1000</f>
+        <v>46.759</v>
+      </c>
       <c r="L17" s="0" t="n">
         <v>1</v>
       </c>
@@ -617,6 +760,10 @@
       <c r="D18" s="0" t="n">
         <v>9547</v>
       </c>
+      <c r="E18" s="0" t="n">
+        <f aca="false">D18/1000</f>
+        <v>9.547</v>
+      </c>
       <c r="F18" s="0" t="n">
         <v>0.999074</v>
       </c>
@@ -629,6 +776,10 @@
       <c r="J18" s="0" t="n">
         <v>103991</v>
       </c>
+      <c r="K18" s="0" t="n">
+        <f aca="false">J18/1000</f>
+        <v>103.991</v>
+      </c>
       <c r="L18" s="0" t="n">
         <v>1</v>
       </c>
@@ -643,6 +794,10 @@
       <c r="D19" s="0" t="n">
         <v>4330</v>
       </c>
+      <c r="E19" s="0" t="n">
+        <f aca="false">D19/1000</f>
+        <v>4.33</v>
+      </c>
       <c r="F19" s="0" t="n">
         <v>0.974999</v>
       </c>
@@ -655,6 +810,10 @@
       <c r="J19" s="0" t="n">
         <v>43325</v>
       </c>
+      <c r="K19" s="0" t="n">
+        <f aca="false">J19/1000</f>
+        <v>43.325</v>
+      </c>
       <c r="L19" s="0" t="n">
         <v>1</v>
       </c>
@@ -669,6 +828,10 @@
       <c r="D20" s="0" t="n">
         <v>4776</v>
       </c>
+      <c r="E20" s="0" t="n">
+        <f aca="false">D20/1000</f>
+        <v>4.776</v>
+      </c>
       <c r="F20" s="0" t="n">
         <v>0.952778</v>
       </c>
@@ -681,6 +844,10 @@
       <c r="J20" s="0" t="n">
         <v>70150</v>
       </c>
+      <c r="K20" s="0" t="n">
+        <f aca="false">J20/1000</f>
+        <v>70.15</v>
+      </c>
       <c r="L20" s="0" t="n">
         <v>0.25</v>
       </c>
@@ -695,6 +862,10 @@
       <c r="D21" s="0" t="n">
         <v>10083</v>
       </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">D21/1000</f>
+        <v>10.083</v>
+      </c>
       <c r="F21" s="0" t="n">
         <v>0.976852</v>
       </c>
@@ -707,6 +878,10 @@
       <c r="J21" s="0" t="n">
         <v>41087</v>
       </c>
+      <c r="K21" s="0" t="n">
+        <f aca="false">J21/1000</f>
+        <v>41.087</v>
+      </c>
       <c r="L21" s="0" t="n">
         <v>1</v>
       </c>
@@ -721,6 +896,10 @@
       <c r="D22" s="0" t="n">
         <v>6461</v>
       </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">D22/1000</f>
+        <v>6.461</v>
+      </c>
       <c r="F22" s="0" t="n">
         <v>0.988889</v>
       </c>
@@ -733,6 +912,10 @@
       <c r="J22" s="0" t="n">
         <v>141102</v>
       </c>
+      <c r="K22" s="0" t="n">
+        <f aca="false">J22/1000</f>
+        <v>141.102</v>
+      </c>
       <c r="L22" s="0" t="n">
         <v>0.166666666666667</v>
       </c>
@@ -747,8 +930,1800 @@
       <c r="D23" s="0" t="n">
         <v>2553</v>
       </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">D23/1000</f>
+        <v>2.553</v>
+      </c>
       <c r="F23" s="0" t="n">
         <v>0.999074</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <f aca="false">AVERAGE(E4:E13)</f>
+        <v>6.1191</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <f aca="false">AVERAGE(F4:F13)</f>
+        <v>0.91666666666</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <f aca="false">AVERAGE(K11:K22)</f>
+        <v>79.17625</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <f aca="false">AVERAGE(L11:L22)</f>
+        <v>0.784722222222222</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <f aca="false">AVERAGE(E14:E23)</f>
+        <v>5.9239</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <f aca="false">AVERAGE(F14:F23)</f>
+        <v>0.9410185</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <f aca="false">AVERAGE(K4:K10)</f>
+        <v>5.41985714285714</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <f aca="false">AVERAGE(L4:L10)</f>
+        <v>0.908972714285714</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>6404</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <f aca="false">D27/1000</f>
+        <v>6.404</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>19369</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <f aca="false">J27/1000</f>
+        <v>19.369</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>6110</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <f aca="false">D28/1000</f>
+        <v>6.11</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>19394</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <f aca="false">J28/1000</f>
+        <v>19.394</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>8253</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">D29/1000</f>
+        <v>8.253</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>26880</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <f aca="false">J29/1000</f>
+        <v>26.88</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>6037</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">D30/1000</f>
+        <v>6.037</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H30" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>70423</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <f aca="false">J30/1000</f>
+        <v>70.423</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>7491</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <f aca="false">D31/1000</f>
+        <v>7.491</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>22037</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <f aca="false">J31/1000</f>
+        <v>22.037</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>7041</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <f aca="false">D32/1000</f>
+        <v>7.041</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0.988888</v>
+      </c>
+      <c r="H32" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>37903</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <f aca="false">J32/1000</f>
+        <v>37.903</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>5455</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <f aca="false">D33/1000</f>
+        <v>5.455</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0.800309</v>
+      </c>
+      <c r="H33" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>26546</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <f aca="false">J33/1000</f>
+        <v>26.546</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>4793</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <f aca="false">D34/1000</f>
+        <v>4.793</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>0.900617</v>
+      </c>
+      <c r="H34" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>206705</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <f aca="false">J34/1000</f>
+        <v>206.705</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>5309</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <f aca="false">D35/1000</f>
+        <v>5.309</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0.960957</v>
+      </c>
+      <c r="H35" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>21896</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <f aca="false">J35/1000</f>
+        <v>21.896</v>
+      </c>
+      <c r="L35" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>5983</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <f aca="false">D36/1000</f>
+        <v>5.983</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0.970833</v>
+      </c>
+      <c r="H36" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>21904</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <f aca="false">J36/1000</f>
+        <v>21.904</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H37" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>7134</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <f aca="false">J37/1000</f>
+        <v>7.134</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>7141</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <f aca="false">J38/1000</f>
+        <v>7.141</v>
+      </c>
+      <c r="L38" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H39" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>182455</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <f aca="false">J39/1000</f>
+        <v>182.455</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H40" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>11072</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <f aca="false">J40/1000</f>
+        <v>11.072</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H41" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>11086</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <f aca="false">J41/1000</f>
+        <v>11.086</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H42" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>7961</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <f aca="false">J42/1000</f>
+        <v>7.961</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>0.944753</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H43" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>7254</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <f aca="false">J43/1000</f>
+        <v>7.254</v>
+      </c>
+      <c r="L43" s="0" t="n">
+        <v>0.936728</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">AVERAGE(E27:E31)</f>
+        <v>6.859</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <f aca="false">AVERAGE(F27:F31)</f>
+        <v>0.9</v>
+      </c>
+      <c r="H44" s="3"/>
+      <c r="K44" s="0" t="n">
+        <f aca="false">AVERAGE(K27:K34)</f>
+        <v>53.657125</v>
+      </c>
+      <c r="L44" s="0" t="n">
+        <f aca="false">AVERAGE(L27:L34)</f>
+        <v>0.854166625</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">AVERAGE(E32:E36)</f>
+        <v>5.7162</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <f aca="false">AVERAGE(F32:F36)</f>
+        <v>0.9243208</v>
+      </c>
+      <c r="H45" s="3"/>
+      <c r="K45" s="0" t="n">
+        <f aca="false">AVERAGE(K35:K42)</f>
+        <v>33.831125</v>
+      </c>
+      <c r="L45" s="0" t="n">
+        <f aca="false">AVERAGE(L35:L42)</f>
+        <v>0.70142725</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B47" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>4101</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <f aca="false">D47/1000</f>
+        <v>4.101</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>0.964815</v>
+      </c>
+      <c r="H47" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <v>16861</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <f aca="false">J47/1000</f>
+        <v>16.861</v>
+      </c>
+      <c r="L47" s="0" t="n">
+        <v>0.940741</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>4113</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <f aca="false">D48/1000</f>
+        <v>4.113</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>0.964815</v>
+      </c>
+      <c r="H48" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I48" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J48" s="0" t="n">
+        <v>19323</v>
+      </c>
+      <c r="K48" s="0" t="n">
+        <f aca="false">J48/1000</f>
+        <v>19.323</v>
+      </c>
+      <c r="L48" s="0" t="n">
+        <v>0.78642</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>6249</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <f aca="false">D49/1000</f>
+        <v>6.249</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>0.878704</v>
+      </c>
+      <c r="H49" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J49" s="0" t="n">
+        <v>13759</v>
+      </c>
+      <c r="K49" s="0" t="n">
+        <f aca="false">J49/1000</f>
+        <v>13.759</v>
+      </c>
+      <c r="L49" s="0" t="n">
+        <v>0.652006</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>2828</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <f aca="false">D50/1000</f>
+        <v>2.828</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>0.950926</v>
+      </c>
+      <c r="H50" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <v>22583</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <f aca="false">J50/1000</f>
+        <v>22.583</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <v>0.477469</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>2893</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <f aca="false">D51/1000</f>
+        <v>2.893</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>0.950926</v>
+      </c>
+      <c r="H51" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>9935</v>
+      </c>
+      <c r="K51" s="0" t="n">
+        <f aca="false">J51/1000</f>
+        <v>9.935</v>
+      </c>
+      <c r="L51" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>3577</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <f aca="false">D52/1000</f>
+        <v>3.577</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>0.914815</v>
+      </c>
+      <c r="H52" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>9945</v>
+      </c>
+      <c r="K52" s="0" t="n">
+        <f aca="false">J52/1000</f>
+        <v>9.945</v>
+      </c>
+      <c r="L52" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>7666</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <f aca="false">D53/1000</f>
+        <v>7.666</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>0.166666</v>
+      </c>
+      <c r="H53" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>518766</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <f aca="false">J53/1000</f>
+        <v>518.766</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>17749</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">D54/1000</f>
+        <v>17.749</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H54" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <v>523021</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <f aca="false">J54/1000</f>
+        <v>523.021</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>8454</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <f aca="false">D55/1000</f>
+        <v>8.454</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H55" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J55" s="0" t="n">
+        <v>525262</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <f aca="false">J55/1000</f>
+        <v>525.262</v>
+      </c>
+      <c r="L55" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>15283</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <f aca="false">D56/1000</f>
+        <v>15.283</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="H56" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J56" s="0" t="n">
+        <v>151095</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <f aca="false">J56/1000</f>
+        <v>151.095</v>
+      </c>
+      <c r="L56" s="0" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>13985</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <f aca="false">D57/1000</f>
+        <v>13.985</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H57" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <v>76428</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <f aca="false">J57/1000</f>
+        <v>76.428</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>10164</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <f aca="false">D58/1000</f>
+        <v>10.164</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="H58" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>53224</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <f aca="false">J58/1000</f>
+        <v>53.224</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H59" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J59" s="0" t="n">
+        <v>69559</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <f aca="false">J59/1000</f>
+        <v>69.559</v>
+      </c>
+      <c r="L59" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H60" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I60" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v>88874</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <f aca="false">J60/1000</f>
+        <v>88.874</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <f aca="false">AVERAGE(E54:E58)</f>
+        <v>13.127</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <f aca="false">AVERAGE(F54:F58)</f>
+        <v>0.332</v>
+      </c>
+      <c r="H61" s="3"/>
+      <c r="K61" s="0" t="n">
+        <f aca="false">AVERAGE(K53:K60)</f>
+        <v>250.778625</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <f aca="false">AVERAGE(L53:L60)</f>
+        <v>0.4479165</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <f aca="false">AVERAGE(E47:E53)</f>
+        <v>4.48957142857143</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <f aca="false">AVERAGE(F47:F53)</f>
+        <v>0.827381</v>
+      </c>
+      <c r="H62" s="3"/>
+      <c r="K62" s="0" t="n">
+        <f aca="false">AVERAGE(K47:K52)</f>
+        <v>15.401</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <f aca="false">AVERAGE(L47:L52)</f>
+        <v>0.716846666666667</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>7439</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <f aca="false">D64/1000</f>
+        <v>7.439</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H64" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J64" s="0" t="n">
+        <v>17511</v>
+      </c>
+      <c r="K64" s="0" t="n">
+        <f aca="false">J64/1000</f>
+        <v>17.511</v>
+      </c>
+      <c r="L64" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>7417</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <f aca="false">D65/1000</f>
+        <v>7.417</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H65" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J65" s="0" t="n">
+        <v>11692</v>
+      </c>
+      <c r="K65" s="0" t="n">
+        <f aca="false">J65/1000</f>
+        <v>11.692</v>
+      </c>
+      <c r="L65" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>5335</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <f aca="false">D66/1000</f>
+        <v>5.335</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H66" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J66" s="0" t="n">
+        <v>11786</v>
+      </c>
+      <c r="K66" s="0" t="n">
+        <f aca="false">J66/1000</f>
+        <v>11.786</v>
+      </c>
+      <c r="L66" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>6976</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <f aca="false">D67/1000</f>
+        <v>6.976</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H67" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I67" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J67" s="0" t="n">
+        <v>13028</v>
+      </c>
+      <c r="K67" s="0" t="n">
+        <f aca="false">J67/1000</f>
+        <v>13.028</v>
+      </c>
+      <c r="L67" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>4316</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <f aca="false">D68/1000</f>
+        <v>4.316</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H68" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I68" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J68" s="0" t="n">
+        <v>8001</v>
+      </c>
+      <c r="K68" s="0" t="n">
+        <f aca="false">J68/1000</f>
+        <v>8.001</v>
+      </c>
+      <c r="L68" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>1566</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <f aca="false">D69/1000</f>
+        <v>1.566</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>0.866666</v>
+      </c>
+      <c r="H69" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J69" s="0" t="n">
+        <v>8009</v>
+      </c>
+      <c r="K69" s="0" t="n">
+        <f aca="false">J69/1000</f>
+        <v>8.009</v>
+      </c>
+      <c r="L69" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>6547</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <f aca="false">D70/1000</f>
+        <v>6.547</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>0.999074</v>
+      </c>
+      <c r="H70" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I70" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J70" s="0" t="n">
+        <v>14623</v>
+      </c>
+      <c r="K70" s="0" t="n">
+        <f aca="false">J70/1000</f>
+        <v>14.623</v>
+      </c>
+      <c r="L70" s="0" t="n">
+        <v>0.91466</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>4946</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <f aca="false">D71/1000</f>
+        <v>4.946</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>0.952778</v>
+      </c>
+      <c r="H71" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I71" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J71" s="0" t="n">
+        <v>8866</v>
+      </c>
+      <c r="K71" s="0" t="n">
+        <f aca="false">J71/1000</f>
+        <v>8.866</v>
+      </c>
+      <c r="L71" s="0" t="n">
+        <v>0.975</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>4178</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <f aca="false">D72/1000</f>
+        <v>4.178</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>0.987037</v>
+      </c>
+      <c r="H72" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J72" s="0" t="n">
+        <v>7795</v>
+      </c>
+      <c r="K72" s="0" t="n">
+        <f aca="false">J72/1000</f>
+        <v>7.795</v>
+      </c>
+      <c r="L72" s="0" t="n">
+        <v>0.958951</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>6277</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <f aca="false">D73/1000</f>
+        <v>6.277</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>0.964815</v>
+      </c>
+      <c r="H73" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J73" s="0" t="n">
+        <v>7346</v>
+      </c>
+      <c r="K73" s="0" t="n">
+        <f aca="false">J73/1000</f>
+        <v>7.346</v>
+      </c>
+      <c r="L73" s="0" t="n">
+        <v>0.976852</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <f aca="false">AVERAGE(E64:E68)</f>
+        <v>6.2966</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <f aca="false">AVERAGE(F64:F68)</f>
+        <v>0.8</v>
+      </c>
+      <c r="K74" s="0" t="n">
+        <f aca="false">AVERAGE(K64:K67)</f>
+        <v>13.50425</v>
+      </c>
+      <c r="L74" s="0" t="n">
+        <f aca="false">AVERAGE(L64:L67)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <f aca="false">AVERAGE(E69:E73)</f>
+        <v>4.7028</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <f aca="false">AVERAGE(F69:F73)</f>
+        <v>0.954074</v>
+      </c>
+      <c r="K75" s="0" t="n">
+        <f aca="false">AVERAGE(K68:K73)</f>
+        <v>9.10666666666667</v>
+      </c>
+      <c r="L75" s="0" t="n">
+        <f aca="false">AVERAGE(L68:L73)</f>
+        <v>0.878317833333333</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B77" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>7583</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <f aca="false">D77/1000</f>
+        <v>7.583</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H77" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I77" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J77" s="0" t="n">
+        <v>143760</v>
+      </c>
+      <c r="K77" s="0" t="n">
+        <f aca="false">J77/1000</f>
+        <v>143.76</v>
+      </c>
+      <c r="L77" s="0" t="n">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>8657</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <f aca="false">D78/1000</f>
+        <v>8.657</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H78" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I78" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J78" s="0" t="n">
+        <v>42565</v>
+      </c>
+      <c r="K78" s="0" t="n">
+        <f aca="false">J78/1000</f>
+        <v>42.565</v>
+      </c>
+      <c r="L78" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>7214</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <f aca="false">D79/1000</f>
+        <v>7.214</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I79" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J79" s="0" t="n">
+        <v>54837</v>
+      </c>
+      <c r="K79" s="0" t="n">
+        <f aca="false">J79/1000</f>
+        <v>54.837</v>
+      </c>
+      <c r="L79" s="0" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>6263</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <f aca="false">D80/1000</f>
+        <v>6.263</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H80" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I80" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J80" s="0" t="n">
+        <v>13396</v>
+      </c>
+      <c r="K80" s="0" t="n">
+        <f aca="false">J80/1000</f>
+        <v>13.396</v>
+      </c>
+      <c r="L80" s="0" t="n">
+        <v>0.950926</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>9614</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <f aca="false">D81/1000</f>
+        <v>9.614</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>0.999074</v>
+      </c>
+      <c r="H81" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I81" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J81" s="0" t="n">
+        <v>8870</v>
+      </c>
+      <c r="K81" s="0" t="n">
+        <f aca="false">J81/1000</f>
+        <v>8.87</v>
+      </c>
+      <c r="L81" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>4606</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <f aca="false">D82/1000</f>
+        <v>4.606</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>0.940741</v>
+      </c>
+      <c r="H82" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I82" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J82" s="0" t="n">
+        <v>8883</v>
+      </c>
+      <c r="K82" s="0" t="n">
+        <f aca="false">J82/1000</f>
+        <v>8.883</v>
+      </c>
+      <c r="L82" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>4743</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <f aca="false">D83/1000</f>
+        <v>4.743</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>0.962963</v>
+      </c>
+      <c r="H83" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I83" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J83" s="0" t="n">
+        <v>12108</v>
+      </c>
+      <c r="K83" s="0" t="n">
+        <f aca="false">J83/1000</f>
+        <v>12.108</v>
+      </c>
+      <c r="L83" s="0" t="n">
+        <v>0.954938</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>4395</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <f aca="false">D84/1000</f>
+        <v>4.395</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>0.987037</v>
+      </c>
+      <c r="H84" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I84" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J84" s="0" t="n">
+        <v>12592</v>
+      </c>
+      <c r="K84" s="0" t="n">
+        <f aca="false">J84/1000</f>
+        <v>12.592</v>
+      </c>
+      <c r="L84" s="0" t="n">
+        <v>0.926697</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>5301</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <f aca="false">D85/1000</f>
+        <v>5.301</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>0.964815</v>
+      </c>
+      <c r="H85" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J85" s="0" t="n">
+        <v>9287</v>
+      </c>
+      <c r="K85" s="0" t="n">
+        <f aca="false">J85/1000</f>
+        <v>9.287</v>
+      </c>
+      <c r="L85" s="0" t="n">
+        <v>0.938889</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <f aca="false">AVERAGE(E77:E80)</f>
+        <v>7.42925</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <f aca="false">AVERAGE(F77:F80)</f>
+        <v>0.875</v>
+      </c>
+      <c r="K86" s="0" t="n">
+        <f aca="false">AVERAGE(K77:K79)</f>
+        <v>80.3873333333333</v>
+      </c>
+      <c r="L86" s="0" t="n">
+        <f aca="false">AVERAGE(L77:L79)</f>
+        <v>0.219444333333333</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <f aca="false">AVERAGE(E81:E85)</f>
+        <v>5.7318</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <f aca="false">AVERAGE(F81:F85)</f>
+        <v>0.970926</v>
+      </c>
+      <c r="K87" s="0" t="n">
+        <f aca="false">AVERAGE(K80:K85)</f>
+        <v>10.856</v>
+      </c>
+      <c r="L87" s="0" t="n">
+        <f aca="false">AVERAGE(L80:L85)</f>
+        <v>0.869315666666667</v>
       </c>
     </row>
   </sheetData>
@@ -760,4 +2735,279 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0357142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>6.1191</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.91666666666</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>5.9239</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.9410185</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>79.17625</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.784722222222222</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>5.41985714285714</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.908972714285714</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>6.859</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>5.7162</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.9243208</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>53.657125</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.854166625</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>33.831125</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.70142725</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>13.127</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.332</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>4.48957142857143</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.827381</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>250.778625</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0.4479165</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>15.401</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.716846666666667</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>6.2966</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>4.7028</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.954074</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>13.50425</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>9.10666666666667</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.878317833333333</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>7.42925</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>5.7318</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.970926</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>80.3873333333333</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0.219444333333333</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>10.856</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.869315666666667</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">AVERAGE(B5:B12)</f>
+        <v>7.96619</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <f aca="false">AVERAGE(C5:C12)</f>
+        <v>0.764733333332</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">AVERAGE(D5:D12)</f>
+        <v>5.31285428571429</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">AVERAGE(E5:E12)</f>
+        <v>0.92354406</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <f aca="false">AVERAGE(F5:F12)</f>
+        <v>95.5007166666667</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">AVERAGE(G5:G12)</f>
+        <v>0.661249936111111</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">AVERAGE(H5:H12)</f>
+        <v>14.9229297619048</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">AVERAGE(I5:I12)</f>
+        <v>0.814976026190476</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update results with questionnaire data and some charts
* See second tab for average time and accuracy charts
</commit_message>
<xml_diff>
--- a/Phase 3 - Experiment/Results.xlsx
+++ b/Phase 3 - Experiment/Results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="49">
   <si>
     <t xml:space="preserve">Experiment Results</t>
   </si>
@@ -32,6 +32,15 @@
     <t xml:space="preserve">TouchBand</t>
   </si>
   <si>
+    <t xml:space="preserve">Post-questionnaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mode</t>
+  </si>
+  <si>
     <t xml:space="preserve">Participant</t>
   </si>
   <si>
@@ -50,12 +59,69 @@
     <t xml:space="preserve">Accuracy</t>
   </si>
   <si>
+    <t xml:space="preserve">Difficultly learning to use wristband</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2,3</t>
+  </si>
+  <si>
     <t xml:space="preserve">scrolling</t>
   </si>
   <si>
     <t xml:space="preserve">zooming</t>
   </si>
   <si>
+    <t xml:space="preserve">touchscreen for scrolling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">touchscreen for zooming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">touchband for scrolling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">touchband for zooming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intuitive scrolling on band</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intuitive zooming on band</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferred for scrolling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">band</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferred for zooming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">touchscreen fatigue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">touchband fatigue</t>
+  </si>
+  <si>
     <t xml:space="preserve">Avg scrolling</t>
   </si>
   <si>
@@ -84,20 +150,40 @@
   </si>
   <si>
     <t xml:space="preserve">Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Std Dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD Touchscreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD Touchband</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scrolling task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zooming task</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -119,17 +205,35 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,7 +278,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -184,6 +288,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,7 +312,808 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Average task completion time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AvgByParticipant!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Touchscreen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AvgByParticipant!$A$19:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Scrolling task</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Zooming task</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AvgByParticipant!$B$19:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.96619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.31285428571429</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AvgByParticipant!$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Touchband</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AvgByParticipant!$A$19:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Scrolling task</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Zooming task</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AvgByParticipant!$C$19:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>95.5007166666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.9229297619048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="30390366"/>
+        <c:axId val="51872361"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="30390366"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="51872361"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51872361"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="30390366"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Average accuracy by task</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AvgByParticipant!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Touchscreen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AvgByParticipant!$A$22:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>scrolling accuracy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>zooming accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AvgByParticipant!$B$22:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.764733333332</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92354406</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AvgByParticipant!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Touchband</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AvgByParticipant!$A$22:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>scrolling accuracy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>zooming accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AvgByParticipant!$C$22:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.661249936111111</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.814976026190476</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="45841745"/>
+        <c:axId val="27257537"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="45841745"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="27257537"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="27257537"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="45841745"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1096560</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>142200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>636480</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>130680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1096560" y="4043520"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>994320</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>532440</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>102960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7214040" y="4015800"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -208,19 +1121,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:X87"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W10" activeCellId="0" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="12.1122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.2040816326531"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="12.1122448979592"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="12.1122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,51 +1150,106 @@
       <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="N2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="S3" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="V3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="X3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>13460</v>
@@ -291,11 +1261,11 @@
       <c r="F4" s="0" t="n">
         <v>0.1666666666</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="5" t="n">
         <v>11</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>4696</v>
@@ -307,13 +1277,41 @@
       <c r="L4" s="0" t="n">
         <v>0.936883</v>
       </c>
+      <c r="N4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>8306</v>
@@ -325,11 +1323,11 @@
       <c r="F5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="5" t="n">
         <v>11</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>5090</v>
@@ -341,13 +1339,41 @@
       <c r="L5" s="0" t="n">
         <v>0.928704</v>
       </c>
+      <c r="N5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="W5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="X5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>4536</v>
@@ -359,11 +1385,11 @@
       <c r="F6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="5" t="n">
         <v>11</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>6043</v>
@@ -375,13 +1401,41 @@
       <c r="L6" s="0" t="n">
         <v>0.95679</v>
       </c>
+      <c r="N6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="X6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>4291</v>
@@ -393,11 +1447,11 @@
       <c r="F7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="5" t="n">
         <v>11</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>5314</v>
@@ -409,13 +1463,38 @@
       <c r="L7" s="0" t="n">
         <v>0.764352</v>
       </c>
+      <c r="N7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="W7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="X7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>5430</v>
@@ -427,11 +1506,11 @@
       <c r="F8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="3" t="n">
+      <c r="H8" s="5" t="n">
         <v>11</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>4300</v>
@@ -443,13 +1522,41 @@
       <c r="L8" s="0" t="n">
         <v>0.986883</v>
       </c>
+      <c r="N8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V8" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="W8" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="X8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>3672</v>
@@ -461,11 +1568,11 @@
       <c r="F9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="3" t="n">
+      <c r="H9" s="5" t="n">
         <v>11</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>7041</v>
@@ -477,13 +1584,38 @@
       <c r="L9" s="0" t="n">
         <v>0.988889</v>
       </c>
+      <c r="N9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V9" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>4266</v>
@@ -495,11 +1627,11 @@
       <c r="F10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="3" t="n">
+      <c r="H10" s="5" t="n">
         <v>11</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>5455</v>
@@ -511,13 +1643,37 @@
       <c r="L10" s="0" t="n">
         <v>0.800308</v>
       </c>
+      <c r="N10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>6606</v>
@@ -533,7 +1689,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>26367</v>
@@ -545,13 +1701,34 @@
       <c r="L11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>6345</v>
@@ -567,7 +1744,7 @@
         <v>11</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>27766</v>
@@ -579,13 +1756,37 @@
       <c r="L12" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>4279</v>
@@ -601,7 +1802,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>38954</v>
@@ -613,13 +1814,34 @@
       <c r="L13" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="N13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="R13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="S13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T13" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>6719</v>
@@ -635,7 +1857,7 @@
         <v>11</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>41198</v>
@@ -649,11 +1871,11 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>5670</v>
@@ -669,7 +1891,7 @@
         <v>11</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>68394</v>
@@ -683,11 +1905,11 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>4699</v>
@@ -703,7 +1925,7 @@
         <v>11</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>301022</v>
@@ -717,11 +1939,11 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>4401</v>
@@ -737,7 +1959,7 @@
         <v>11</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>46759</v>
@@ -751,11 +1973,11 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>9547</v>
@@ -771,7 +1993,7 @@
         <v>11</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>103991</v>
@@ -785,11 +2007,11 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>4330</v>
@@ -805,7 +2027,7 @@
         <v>11</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>43325</v>
@@ -819,11 +2041,11 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>4776</v>
@@ -839,7 +2061,7 @@
         <v>11</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>70150</v>
@@ -853,11 +2075,11 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>10083</v>
@@ -873,7 +2095,7 @@
         <v>11</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>41087</v>
@@ -887,11 +2109,11 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>6461</v>
@@ -907,7 +2129,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>141102</v>
@@ -921,11 +2143,11 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="3" t="n">
+      <c r="B23" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>2553</v>
@@ -939,8 +2161,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3" t="s">
-        <v>11</v>
+      <c r="B24" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E24" s="0" t="n">
         <f aca="false">AVERAGE(E4:E13)</f>
@@ -960,8 +2182,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="3" t="s">
-        <v>12</v>
+      <c r="B25" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="E25" s="0" t="n">
         <f aca="false">AVERAGE(E14:E23)</f>
@@ -981,17 +2203,17 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="3"/>
+      <c r="B26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B27" s="3" t="n">
+      <c r="B27" s="5" t="n">
         <v>16</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>6404</v>
@@ -1003,11 +2225,11 @@
       <c r="F27" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H27" s="3" t="n">
+      <c r="H27" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>19369</v>
@@ -1021,11 +2243,11 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="5" t="n">
         <v>16</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>6110</v>
@@ -1037,11 +2259,11 @@
       <c r="F28" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H28" s="3" t="n">
+      <c r="H28" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>19394</v>
@@ -1055,11 +2277,11 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="3" t="n">
+      <c r="B29" s="5" t="n">
         <v>16</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>8253</v>
@@ -1071,11 +2293,11 @@
       <c r="F29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H29" s="3" t="n">
+      <c r="H29" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>26880</v>
@@ -1089,11 +2311,11 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="3" t="n">
+      <c r="B30" s="5" t="n">
         <v>16</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>6037</v>
@@ -1105,11 +2327,11 @@
       <c r="F30" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="H30" s="3" t="n">
+      <c r="H30" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>70423</v>
@@ -1123,11 +2345,11 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="3" t="n">
+      <c r="B31" s="5" t="n">
         <v>16</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>7491</v>
@@ -1139,11 +2361,11 @@
       <c r="F31" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H31" s="3" t="n">
+      <c r="H31" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J31" s="0" t="n">
         <v>22037</v>
@@ -1157,11 +2379,11 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="3" t="n">
+      <c r="B32" s="5" t="n">
         <v>12</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>7041</v>
@@ -1173,11 +2395,11 @@
       <c r="F32" s="0" t="n">
         <v>0.988888</v>
       </c>
-      <c r="H32" s="3" t="n">
+      <c r="H32" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>37903</v>
@@ -1191,11 +2413,11 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="3" t="n">
+      <c r="B33" s="5" t="n">
         <v>12</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>5455</v>
@@ -1207,11 +2429,11 @@
       <c r="F33" s="0" t="n">
         <v>0.800309</v>
       </c>
-      <c r="H33" s="3" t="n">
+      <c r="H33" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>26546</v>
@@ -1225,11 +2447,11 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="3" t="n">
+      <c r="B34" s="5" t="n">
         <v>12</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>4793</v>
@@ -1241,11 +2463,11 @@
       <c r="F34" s="0" t="n">
         <v>0.900617</v>
       </c>
-      <c r="H34" s="3" t="n">
+      <c r="H34" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>206705</v>
@@ -1259,11 +2481,11 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="3" t="n">
+      <c r="B35" s="5" t="n">
         <v>12</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>5309</v>
@@ -1275,11 +2497,11 @@
       <c r="F35" s="0" t="n">
         <v>0.960957</v>
       </c>
-      <c r="H35" s="3" t="n">
+      <c r="H35" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>21896</v>
@@ -1293,11 +2515,11 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="3" t="n">
+      <c r="B36" s="5" t="n">
         <v>12</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>5983</v>
@@ -1309,11 +2531,11 @@
       <c r="F36" s="0" t="n">
         <v>0.970833</v>
       </c>
-      <c r="H36" s="3" t="n">
+      <c r="H36" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J36" s="0" t="n">
         <v>21904</v>
@@ -1327,11 +2549,11 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H37" s="3" t="n">
+      <c r="H37" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J37" s="0" t="n">
         <v>7134</v>
@@ -1345,11 +2567,11 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="3" t="n">
+      <c r="H38" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>7141</v>
@@ -1363,11 +2585,11 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H39" s="3" t="n">
+      <c r="H39" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>182455</v>
@@ -1381,11 +2603,11 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="3" t="n">
+      <c r="H40" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>11072</v>
@@ -1399,11 +2621,11 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="3" t="n">
+      <c r="H41" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J41" s="0" t="n">
         <v>11086</v>
@@ -1417,11 +2639,11 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="3" t="n">
+      <c r="H42" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J42" s="0" t="n">
         <v>7961</v>
@@ -1435,11 +2657,11 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="3" t="n">
+      <c r="H43" s="5" t="n">
         <v>13</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>7254</v>
@@ -1453,8 +2675,8 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="3" t="s">
-        <v>11</v>
+      <c r="B44" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E44" s="0" t="n">
         <f aca="false">AVERAGE(E27:E31)</f>
@@ -1464,7 +2686,7 @@
         <f aca="false">AVERAGE(F27:F31)</f>
         <v>0.9</v>
       </c>
-      <c r="H44" s="3"/>
+      <c r="H44" s="5"/>
       <c r="K44" s="0" t="n">
         <f aca="false">AVERAGE(K27:K34)</f>
         <v>53.657125</v>
@@ -1475,8 +2697,8 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="3" t="s">
-        <v>12</v>
+      <c r="B45" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="E45" s="0" t="n">
         <f aca="false">AVERAGE(E32:E36)</f>
@@ -1486,7 +2708,7 @@
         <f aca="false">AVERAGE(F32:F36)</f>
         <v>0.9243208</v>
       </c>
-      <c r="H45" s="3"/>
+      <c r="H45" s="5"/>
       <c r="K45" s="0" t="n">
         <f aca="false">AVERAGE(K35:K42)</f>
         <v>33.831125</v>
@@ -1497,17 +2719,17 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="3"/>
+      <c r="H46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B47" s="3" t="n">
+      <c r="B47" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>4101</v>
@@ -1519,11 +2741,11 @@
       <c r="F47" s="0" t="n">
         <v>0.964815</v>
       </c>
-      <c r="H47" s="3" t="n">
+      <c r="H47" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J47" s="0" t="n">
         <v>16861</v>
@@ -1537,11 +2759,11 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="3" t="n">
+      <c r="B48" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>4113</v>
@@ -1553,11 +2775,11 @@
       <c r="F48" s="0" t="n">
         <v>0.964815</v>
       </c>
-      <c r="H48" s="3" t="n">
+      <c r="H48" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J48" s="0" t="n">
         <v>19323</v>
@@ -1571,11 +2793,11 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="3" t="n">
+      <c r="B49" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>6249</v>
@@ -1587,11 +2809,11 @@
       <c r="F49" s="0" t="n">
         <v>0.878704</v>
       </c>
-      <c r="H49" s="3" t="n">
+      <c r="H49" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J49" s="0" t="n">
         <v>13759</v>
@@ -1605,11 +2827,11 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="3" t="n">
+      <c r="B50" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>2828</v>
@@ -1621,11 +2843,11 @@
       <c r="F50" s="0" t="n">
         <v>0.950926</v>
       </c>
-      <c r="H50" s="3" t="n">
+      <c r="H50" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J50" s="0" t="n">
         <v>22583</v>
@@ -1639,11 +2861,11 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="3" t="n">
+      <c r="B51" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>2893</v>
@@ -1655,11 +2877,11 @@
       <c r="F51" s="0" t="n">
         <v>0.950926</v>
       </c>
-      <c r="H51" s="3" t="n">
+      <c r="H51" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J51" s="0" t="n">
         <v>9935</v>
@@ -1673,11 +2895,11 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="3" t="n">
+      <c r="B52" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>3577</v>
@@ -1689,11 +2911,11 @@
       <c r="F52" s="0" t="n">
         <v>0.914815</v>
       </c>
-      <c r="H52" s="3" t="n">
+      <c r="H52" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J52" s="0" t="n">
         <v>9945</v>
@@ -1707,11 +2929,11 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="3" t="n">
+      <c r="B53" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>7666</v>
@@ -1723,11 +2945,11 @@
       <c r="F53" s="0" t="n">
         <v>0.166666</v>
       </c>
-      <c r="H53" s="3" t="n">
+      <c r="H53" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J53" s="0" t="n">
         <v>518766</v>
@@ -1741,11 +2963,11 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="3" t="n">
+      <c r="B54" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>17749</v>
@@ -1757,11 +2979,11 @@
       <c r="F54" s="0" t="n">
         <v>0.25</v>
       </c>
-      <c r="H54" s="3" t="n">
+      <c r="H54" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J54" s="0" t="n">
         <v>523021</v>
@@ -1775,11 +2997,11 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="3" t="n">
+      <c r="B55" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>8454</v>
@@ -1791,11 +3013,11 @@
       <c r="F55" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="H55" s="3" t="n">
+      <c r="H55" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J55" s="0" t="n">
         <v>525262</v>
@@ -1809,11 +3031,11 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="3" t="n">
+      <c r="B56" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>15283</v>
@@ -1825,11 +3047,11 @@
       <c r="F56" s="0" t="n">
         <v>0.33</v>
       </c>
-      <c r="H56" s="3" t="n">
+      <c r="H56" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J56" s="0" t="n">
         <v>151095</v>
@@ -1843,11 +3065,11 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="3" t="n">
+      <c r="B57" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>13985</v>
@@ -1859,11 +3081,11 @@
       <c r="F57" s="0" t="n">
         <v>0.25</v>
       </c>
-      <c r="H57" s="3" t="n">
+      <c r="H57" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J57" s="0" t="n">
         <v>76428</v>
@@ -1877,11 +3099,11 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="3" t="n">
+      <c r="B58" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>10164</v>
@@ -1893,11 +3115,11 @@
       <c r="F58" s="0" t="n">
         <v>0.33</v>
       </c>
-      <c r="H58" s="3" t="n">
+      <c r="H58" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J58" s="0" t="n">
         <v>53224</v>
@@ -1911,11 +3133,11 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H59" s="3" t="n">
+      <c r="H59" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J59" s="0" t="n">
         <v>69559</v>
@@ -1929,11 +3151,11 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H60" s="3" t="n">
+      <c r="H60" s="5" t="n">
         <v>14</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J60" s="0" t="n">
         <v>88874</v>
@@ -1947,8 +3169,8 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="3" t="s">
-        <v>11</v>
+      <c r="B61" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E61" s="0" t="n">
         <f aca="false">AVERAGE(E54:E58)</f>
@@ -1958,7 +3180,7 @@
         <f aca="false">AVERAGE(F54:F58)</f>
         <v>0.332</v>
       </c>
-      <c r="H61" s="3"/>
+      <c r="H61" s="5"/>
       <c r="K61" s="0" t="n">
         <f aca="false">AVERAGE(K53:K60)</f>
         <v>250.778625</v>
@@ -1969,8 +3191,8 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="3" t="s">
-        <v>12</v>
+      <c r="B62" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="E62" s="0" t="n">
         <f aca="false">AVERAGE(E47:E53)</f>
@@ -1980,7 +3202,7 @@
         <f aca="false">AVERAGE(F47:F53)</f>
         <v>0.827381</v>
       </c>
-      <c r="H62" s="3"/>
+      <c r="H62" s="5"/>
       <c r="K62" s="0" t="n">
         <f aca="false">AVERAGE(K47:K52)</f>
         <v>15.401</v>
@@ -1994,11 +3216,11 @@
       <c r="A64" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B64" s="3" t="n">
+      <c r="B64" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>7439</v>
@@ -2010,11 +3232,11 @@
       <c r="F64" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="H64" s="3" t="n">
+      <c r="H64" s="5" t="n">
         <v>21</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J64" s="0" t="n">
         <v>17511</v>
@@ -2028,11 +3250,11 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="3" t="n">
+      <c r="B65" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>7417</v>
@@ -2044,11 +3266,11 @@
       <c r="F65" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H65" s="3" t="n">
+      <c r="H65" s="5" t="n">
         <v>21</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J65" s="0" t="n">
         <v>11692</v>
@@ -2062,11 +3284,11 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="3" t="n">
+      <c r="B66" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>5335</v>
@@ -2078,11 +3300,11 @@
       <c r="F66" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="H66" s="3" t="n">
+      <c r="H66" s="5" t="n">
         <v>21</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J66" s="0" t="n">
         <v>11786</v>
@@ -2096,11 +3318,11 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="3" t="n">
+      <c r="B67" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>6976</v>
@@ -2112,11 +3334,11 @@
       <c r="F67" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H67" s="3" t="n">
+      <c r="H67" s="5" t="n">
         <v>21</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J67" s="0" t="n">
         <v>13028</v>
@@ -2130,11 +3352,11 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="3" t="n">
+      <c r="B68" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>4316</v>
@@ -2146,11 +3368,11 @@
       <c r="F68" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H68" s="3" t="n">
+      <c r="H68" s="5" t="n">
         <v>21</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J68" s="0" t="n">
         <v>8001</v>
@@ -2164,11 +3386,11 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="3" t="n">
+      <c r="B69" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>1566</v>
@@ -2180,11 +3402,11 @@
       <c r="F69" s="0" t="n">
         <v>0.866666</v>
       </c>
-      <c r="H69" s="3" t="n">
+      <c r="H69" s="5" t="n">
         <v>21</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J69" s="0" t="n">
         <v>8009</v>
@@ -2198,11 +3420,11 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="3" t="n">
+      <c r="B70" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>6547</v>
@@ -2214,11 +3436,11 @@
       <c r="F70" s="0" t="n">
         <v>0.999074</v>
       </c>
-      <c r="H70" s="3" t="n">
+      <c r="H70" s="5" t="n">
         <v>21</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J70" s="0" t="n">
         <v>14623</v>
@@ -2232,11 +3454,11 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="3" t="n">
+      <c r="B71" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>4946</v>
@@ -2248,11 +3470,11 @@
       <c r="F71" s="0" t="n">
         <v>0.952778</v>
       </c>
-      <c r="H71" s="3" t="n">
+      <c r="H71" s="5" t="n">
         <v>21</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J71" s="0" t="n">
         <v>8866</v>
@@ -2266,11 +3488,11 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="3" t="n">
+      <c r="B72" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>4178</v>
@@ -2282,11 +3504,11 @@
       <c r="F72" s="0" t="n">
         <v>0.987037</v>
       </c>
-      <c r="H72" s="3" t="n">
+      <c r="H72" s="5" t="n">
         <v>21</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J72" s="0" t="n">
         <v>7795</v>
@@ -2300,11 +3522,11 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="3" t="n">
+      <c r="B73" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>6277</v>
@@ -2316,11 +3538,11 @@
       <c r="F73" s="0" t="n">
         <v>0.964815</v>
       </c>
-      <c r="H73" s="3" t="n">
+      <c r="H73" s="5" t="n">
         <v>21</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J73" s="0" t="n">
         <v>7346</v>
@@ -2334,8 +3556,8 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="3" t="s">
-        <v>11</v>
+      <c r="B74" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E74" s="0" t="n">
         <f aca="false">AVERAGE(E64:E68)</f>
@@ -2355,8 +3577,8 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="3" t="s">
-        <v>12</v>
+      <c r="B75" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="E75" s="0" t="n">
         <f aca="false">AVERAGE(E69:E73)</f>
@@ -2379,11 +3601,11 @@
       <c r="A77" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B77" s="3" t="n">
+      <c r="B77" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>7583</v>
@@ -2395,11 +3617,11 @@
       <c r="F77" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="H77" s="3" t="n">
+      <c r="H77" s="5" t="n">
         <v>24</v>
       </c>
       <c r="I77" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J77" s="0" t="n">
         <v>143760</v>
@@ -2413,11 +3635,11 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="3" t="n">
+      <c r="B78" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>8657</v>
@@ -2429,11 +3651,11 @@
       <c r="F78" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H78" s="3" t="n">
+      <c r="H78" s="5" t="n">
         <v>24</v>
       </c>
       <c r="I78" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J78" s="0" t="n">
         <v>42565</v>
@@ -2447,11 +3669,11 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="3" t="n">
+      <c r="B79" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D79" s="0" t="n">
         <v>7214</v>
@@ -2463,11 +3685,11 @@
       <c r="F79" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H79" s="3" t="n">
+      <c r="H79" s="5" t="n">
         <v>24</v>
       </c>
       <c r="I79" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J79" s="0" t="n">
         <v>54837</v>
@@ -2481,11 +3703,11 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="3" t="n">
+      <c r="B80" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>6263</v>
@@ -2497,11 +3719,11 @@
       <c r="F80" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H80" s="3" t="n">
+      <c r="H80" s="5" t="n">
         <v>24</v>
       </c>
       <c r="I80" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J80" s="0" t="n">
         <v>13396</v>
@@ -2515,11 +3737,11 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="3" t="n">
+      <c r="B81" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>9614</v>
@@ -2531,11 +3753,11 @@
       <c r="F81" s="0" t="n">
         <v>0.999074</v>
       </c>
-      <c r="H81" s="3" t="n">
+      <c r="H81" s="5" t="n">
         <v>24</v>
       </c>
       <c r="I81" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J81" s="0" t="n">
         <v>8870</v>
@@ -2549,11 +3771,11 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="3" t="n">
+      <c r="B82" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>4606</v>
@@ -2565,11 +3787,11 @@
       <c r="F82" s="0" t="n">
         <v>0.940741</v>
       </c>
-      <c r="H82" s="3" t="n">
+      <c r="H82" s="5" t="n">
         <v>24</v>
       </c>
       <c r="I82" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J82" s="0" t="n">
         <v>8883</v>
@@ -2583,11 +3805,11 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="3" t="n">
+      <c r="B83" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>4743</v>
@@ -2599,11 +3821,11 @@
       <c r="F83" s="0" t="n">
         <v>0.962963</v>
       </c>
-      <c r="H83" s="3" t="n">
+      <c r="H83" s="5" t="n">
         <v>24</v>
       </c>
       <c r="I83" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J83" s="0" t="n">
         <v>12108</v>
@@ -2617,11 +3839,11 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="3" t="n">
+      <c r="B84" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>4395</v>
@@ -2633,11 +3855,11 @@
       <c r="F84" s="0" t="n">
         <v>0.987037</v>
       </c>
-      <c r="H84" s="3" t="n">
+      <c r="H84" s="5" t="n">
         <v>24</v>
       </c>
       <c r="I84" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J84" s="0" t="n">
         <v>12592</v>
@@ -2651,11 +3873,11 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="3" t="n">
+      <c r="B85" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>5301</v>
@@ -2667,11 +3889,11 @@
       <c r="F85" s="0" t="n">
         <v>0.964815</v>
       </c>
-      <c r="H85" s="3" t="n">
+      <c r="H85" s="5" t="n">
         <v>24</v>
       </c>
       <c r="I85" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J85" s="0" t="n">
         <v>9287</v>
@@ -2685,8 +3907,8 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="3" t="s">
-        <v>11</v>
+      <c r="B86" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E86" s="0" t="n">
         <f aca="false">AVERAGE(E77:E80)</f>
@@ -2706,8 +3928,8 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="3" t="s">
-        <v>12</v>
+      <c r="B87" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="E87" s="0" t="n">
         <f aca="false">AVERAGE(E81:E85)</f>
@@ -2742,29 +3964,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0357142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9540816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.8214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3520408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="12.1122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,36 +3994,36 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2966,7 +4188,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B14" s="0" t="n">
         <f aca="false">AVERAGE(B5:B12)</f>
@@ -3001,13 +4223,144 @@
         <v>0.814976026190476</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">STDEV(B5:B9)</f>
+        <v>2.93033301656996</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">STDEV(C5:C9)</f>
+        <v>0.245988527283386</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">STDEV(D5:D9)</f>
+        <v>0.663615294444309</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">STDEV(E5:E9)</f>
+        <v>0.0564145791473091</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <f aca="false">STDEV(F5:F9)</f>
+        <v>90.9401425299782</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">STDEV(G5:G9)</f>
+        <v>0.319341981926465</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">STDEV(H5:H9)</f>
+        <v>11.1627239238309</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">STDEV(I5:I9)</f>
+        <v>0.097881374897099</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>7.96619</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>95.5007166666667</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>2.93033301656996</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>90.9401425299782</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>5.31285428571429</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>14.9229297619048</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0.663615294444309</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>11.1627239238309</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0.764733333332</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0.661249936111111</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0.245988527283386</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0.319341981926465</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0.92354406</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>0.814976026190476</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0.0564145791473091</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.097881374897099</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated results spreadsheet with latest data and updated charts
</commit_message>
<xml_diff>
--- a/Phase 3 - Experiment/Results.xlsx
+++ b/Phase 3 - Experiment/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="58">
   <si>
     <t xml:space="preserve">Experiment Results</t>
   </si>
@@ -122,6 +122,33 @@
     <t xml:space="preserve">touchband fatigue</t>
   </si>
   <si>
+    <t xml:space="preserve">Pre-questionnaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">undergrad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use of smartwatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">never</t>
+  </si>
+  <si>
     <t xml:space="preserve">Avg scrolling</t>
   </si>
   <si>
@@ -178,7 +205,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -222,16 +249,24 @@
     </font>
     <font>
       <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -278,7 +313,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -300,6 +335,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -375,7 +414,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -448,6 +487,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -476,10 +516,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>7.96619</c:v>
+                  <c:v>16.6052979166667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.31285428571429</c:v>
+                  <c:v>5.09841259157509</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -509,6 +549,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -537,10 +578,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>95.5007166666667</c:v>
+                  <c:v>72.5641815705128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.9229297619048</c:v>
+                  <c:v>11.3317723214286</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -548,11 +589,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="30390366"/>
-        <c:axId val="51872361"/>
+        <c:axId val="31065923"/>
+        <c:axId val="75486304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="30390366"/>
+        <c:axId val="31065923"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,14 +628,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51872361"/>
+        <c:crossAx val="75486304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51872361"/>
+        <c:axId val="75486304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,7 +688,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -676,7 +717,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30390366"/>
+        <c:crossAx val="31065923"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -713,7 +754,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -786,6 +827,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -814,10 +856,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.764733333332</c:v>
+                  <c:v>0.786638874999167</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.92354406</c:v>
+                  <c:v>0.91312424514652</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -847,6 +889,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -875,10 +918,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.661249936111111</c:v>
+                  <c:v>0.683725317040598</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.814976026190476</c:v>
+                  <c:v>0.802445843005952</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -886,11 +929,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="45841745"/>
-        <c:axId val="27257537"/>
+        <c:axId val="13664136"/>
+        <c:axId val="41886209"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45841745"/>
+        <c:axId val="13664136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -925,14 +968,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27257537"/>
+        <c:crossAx val="41886209"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27257537"/>
+        <c:axId val="41886209"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -985,7 +1028,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1014,7 +1057,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45841745"/>
+        <c:crossAx val="13664136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1062,9 +1105,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>636480</xdr:colOff>
+      <xdr:colOff>635760</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1073,7 +1116,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1096560" y="4043520"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="6374880" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1092,9 +1135,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>532440</xdr:colOff>
+      <xdr:colOff>531720</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>102960</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1102,8 +1145,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7214040" y="4015800"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="7830000" y="4015800"/>
+        <a:ext cx="6357960" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1121,21 +1164,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X87"/>
+  <dimension ref="A1:Y149"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W10" activeCellId="0" sqref="W10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L149" activeCellId="0" sqref="L149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="12.1122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.2040816326531"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="12.1122448979592"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="12.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0663265306122"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="13.1938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="13.1938775510204"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="31.1632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="13.1938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,10 +1214,16 @@
       <c r="T2" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="U2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="W2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="X2" s="0" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1233,15 +1282,15 @@
       <c r="T3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="V3" s="3" t="n">
+      <c r="W3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="X3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
@@ -1298,15 +1347,15 @@
       <c r="T4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="V4" s="3" t="n">
+      <c r="W4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="X4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="5" t="n">
         <v>9</v>
       </c>
@@ -1360,15 +1409,15 @@
       <c r="T5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="V5" s="3" t="n">
-        <v>3</v>
-      </c>
       <c r="W5" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="X5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="X5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="5" t="n">
         <v>9</v>
       </c>
@@ -1422,15 +1471,15 @@
       <c r="T6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="V6" s="3" t="n">
+      <c r="W6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="X6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="5" t="n">
         <v>9</v>
       </c>
@@ -1481,15 +1530,15 @@
       <c r="T7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="V7" s="3" t="n">
-        <v>4</v>
-      </c>
       <c r="W7" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="X7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="X7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="5" t="n">
         <v>9</v>
       </c>
@@ -1543,15 +1592,15 @@
       <c r="T8" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="V8" s="3" t="n">
+      <c r="W8" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="W8" s="3" t="n">
+      <c r="X8" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="X8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5" t="n">
         <v>9</v>
       </c>
@@ -1602,15 +1651,15 @@
       <c r="T9" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="V9" s="3" t="n">
+      <c r="W9" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="W9" s="3" t="s">
+      <c r="X9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="X9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5" t="n">
         <v>9</v>
       </c>
@@ -1664,11 +1713,11 @@
       <c r="T10" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="5" t="n">
         <v>9</v>
       </c>
@@ -1719,11 +1768,11 @@
       <c r="T11" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5" t="n">
         <v>9</v>
       </c>
@@ -1777,11 +1826,11 @@
       <c r="T12" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="5" t="n">
         <v>9</v>
       </c>
@@ -1836,7 +1885,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5" t="n">
         <v>9</v>
       </c>
@@ -1870,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="5" t="n">
         <v>9</v>
       </c>
@@ -1903,8 +1952,35 @@
       <c r="L15" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="5" t="n">
         <v>9</v>
       </c>
@@ -1937,8 +2013,26 @@
       <c r="L16" s="0" t="n">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="S16" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="5" t="n">
         <v>9</v>
       </c>
@@ -1971,8 +2065,26 @@
       <c r="L17" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="P17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q17" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="R17" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="S17" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="5" t="n">
         <v>9</v>
       </c>
@@ -2005,8 +2117,26 @@
       <c r="L18" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="5" t="n">
         <v>9</v>
       </c>
@@ -2040,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="5" t="n">
         <v>9</v>
       </c>
@@ -2074,7 +2204,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="5" t="n">
         <v>9</v>
       </c>
@@ -2108,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="5" t="n">
         <v>9</v>
       </c>
@@ -2142,7 +2272,7 @@
         <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="5" t="n">
         <v>9</v>
       </c>
@@ -2162,7 +2292,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E24" s="0" t="n">
         <f aca="false">AVERAGE(E4:E13)</f>
@@ -2183,7 +2313,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E25" s="0" t="n">
         <f aca="false">AVERAGE(E14:E23)</f>
@@ -2205,7 +2335,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>2</v>
       </c>
@@ -2242,7 +2372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="5" t="n">
         <v>16</v>
       </c>
@@ -2276,7 +2406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="5" t="n">
         <v>16</v>
       </c>
@@ -2310,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="5" t="n">
         <v>16</v>
       </c>
@@ -2344,7 +2474,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="5" t="n">
         <v>16</v>
       </c>
@@ -2378,7 +2508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="5" t="n">
         <v>12</v>
       </c>
@@ -2412,7 +2542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="5" t="n">
         <v>12</v>
       </c>
@@ -2446,7 +2576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="5" t="n">
         <v>12</v>
       </c>
@@ -2480,7 +2610,7 @@
         <v>0.333333</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="5" t="n">
         <v>12</v>
       </c>
@@ -2514,7 +2644,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="5" t="n">
         <v>12</v>
       </c>
@@ -2548,7 +2678,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H37" s="5" t="n">
         <v>13</v>
       </c>
@@ -2566,7 +2696,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H38" s="5" t="n">
         <v>13</v>
       </c>
@@ -2584,7 +2714,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H39" s="5" t="n">
         <v>13</v>
       </c>
@@ -2602,7 +2732,7 @@
         <v>0.333333</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H40" s="5" t="n">
         <v>13</v>
       </c>
@@ -2620,7 +2750,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H41" s="5" t="n">
         <v>13</v>
       </c>
@@ -2638,7 +2768,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H42" s="5" t="n">
         <v>13</v>
       </c>
@@ -2656,7 +2786,7 @@
         <v>0.944753</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H43" s="5" t="n">
         <v>13</v>
       </c>
@@ -2674,9 +2804,9 @@
         <v>0.936728</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E44" s="0" t="n">
         <f aca="false">AVERAGE(E27:E31)</f>
@@ -2696,9 +2826,9 @@
         <v>0.854166625</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E45" s="0" t="n">
         <f aca="false">AVERAGE(E32:E36)</f>
@@ -2721,7 +2851,7 @@
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H46" s="5"/>
     </row>
-    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>3</v>
       </c>
@@ -2758,7 +2888,7 @@
         <v>0.940741</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="5" t="n">
         <v>15</v>
       </c>
@@ -2792,7 +2922,7 @@
         <v>0.78642</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="5" t="n">
         <v>15</v>
       </c>
@@ -2826,7 +2956,7 @@
         <v>0.652006</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="5" t="n">
         <v>15</v>
       </c>
@@ -2860,7 +2990,7 @@
         <v>0.477469</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="5" t="n">
         <v>15</v>
       </c>
@@ -2894,7 +3024,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="5" t="n">
         <v>15</v>
       </c>
@@ -2928,7 +3058,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="5" t="n">
         <v>15</v>
       </c>
@@ -2962,7 +3092,7 @@
         <v>0.333333</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="5" t="n">
         <v>15</v>
       </c>
@@ -2996,7 +3126,7 @@
         <v>0.333333</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="5" t="n">
         <v>15</v>
       </c>
@@ -3030,7 +3160,7 @@
         <v>0.333333</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="5" t="n">
         <v>15</v>
       </c>
@@ -3064,7 +3194,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="5" t="n">
         <v>15</v>
       </c>
@@ -3098,7 +3228,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="5" t="n">
         <v>15</v>
       </c>
@@ -3132,7 +3262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H59" s="5" t="n">
         <v>14</v>
       </c>
@@ -3150,7 +3280,7 @@
         <v>0.333333</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H60" s="5" t="n">
         <v>14</v>
       </c>
@@ -3168,9 +3298,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E61" s="0" t="n">
         <f aca="false">AVERAGE(E54:E58)</f>
@@ -3190,9 +3320,9 @@
         <v>0.4479165</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E62" s="0" t="n">
         <f aca="false">AVERAGE(E47:E53)</f>
@@ -3212,7 +3342,7 @@
         <v>0.716846666666667</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>4</v>
       </c>
@@ -3249,7 +3379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="5" t="n">
         <v>20</v>
       </c>
@@ -3283,7 +3413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="5" t="n">
         <v>20</v>
       </c>
@@ -3317,7 +3447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="5" t="n">
         <v>20</v>
       </c>
@@ -3351,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="5" t="n">
         <v>20</v>
       </c>
@@ -3385,7 +3515,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="5" t="n">
         <v>20</v>
       </c>
@@ -3419,7 +3549,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="5" t="n">
         <v>20</v>
       </c>
@@ -3453,7 +3583,7 @@
         <v>0.91466</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="5" t="n">
         <v>20</v>
       </c>
@@ -3487,7 +3617,7 @@
         <v>0.975</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="5" t="n">
         <v>20</v>
       </c>
@@ -3521,7 +3651,7 @@
         <v>0.958951</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="5" t="n">
         <v>20</v>
       </c>
@@ -3555,9 +3685,9 @@
         <v>0.976852</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E74" s="0" t="n">
         <f aca="false">AVERAGE(E64:E68)</f>
@@ -3576,9 +3706,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E75" s="0" t="n">
         <f aca="false">AVERAGE(E69:E73)</f>
@@ -3597,7 +3727,7 @@
         <v>0.878317833333333</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>5</v>
       </c>
@@ -3634,7 +3764,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="5" t="n">
         <v>25</v>
       </c>
@@ -3668,7 +3798,7 @@
         <v>0.333333</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="5" t="n">
         <v>25</v>
       </c>
@@ -3702,7 +3832,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="5" t="n">
         <v>25</v>
       </c>
@@ -3736,7 +3866,7 @@
         <v>0.950926</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="5" t="n">
         <v>25</v>
       </c>
@@ -3770,7 +3900,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="5" t="n">
         <v>25</v>
       </c>
@@ -3804,7 +3934,7 @@
         <v>0.722222</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="5" t="n">
         <v>25</v>
       </c>
@@ -3838,7 +3968,7 @@
         <v>0.954938</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="5" t="n">
         <v>25</v>
       </c>
@@ -3872,7 +4002,7 @@
         <v>0.926697</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="5" t="n">
         <v>25</v>
       </c>
@@ -3906,9 +4036,9 @@
         <v>0.938889</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E86" s="0" t="n">
         <f aca="false">AVERAGE(E77:E80)</f>
@@ -3927,9 +4057,9 @@
         <v>0.219444333333333</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E87" s="0" t="n">
         <f aca="false">AVERAGE(E81:E85)</f>
@@ -3946,6 +4076,1772 @@
       <c r="L87" s="0" t="n">
         <f aca="false">AVERAGE(L80:L85)</f>
         <v>0.869315666666667</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="5"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B89" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>7537</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <f aca="false">D89/1000</f>
+        <v>7.537</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H89" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I89" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J89" s="0" t="n">
+        <v>5942</v>
+      </c>
+      <c r="K89" s="0" t="n">
+        <f aca="false">J89/1000</f>
+        <v>5.942</v>
+      </c>
+      <c r="L89" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>5925</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <f aca="false">D90/1000</f>
+        <v>5.925</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H90" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I90" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J90" s="0" t="n">
+        <v>2490</v>
+      </c>
+      <c r="K90" s="0" t="n">
+        <f aca="false">J90/1000</f>
+        <v>2.49</v>
+      </c>
+      <c r="L90" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>107975</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <f aca="false">D91/1000</f>
+        <v>107.975</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H91" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I91" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J91" s="0" t="n">
+        <v>6015</v>
+      </c>
+      <c r="K91" s="0" t="n">
+        <f aca="false">J91/1000</f>
+        <v>6.015</v>
+      </c>
+      <c r="L91" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>5941</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <f aca="false">D92/1000</f>
+        <v>5.941</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H92" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I92" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J92" s="0" t="n">
+        <v>5746</v>
+      </c>
+      <c r="K92" s="0" t="n">
+        <f aca="false">J92/1000</f>
+        <v>5.746</v>
+      </c>
+      <c r="L92" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>4147</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <f aca="false">D93/1000</f>
+        <v>4.147</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H93" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I93" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J93" s="0" t="n">
+        <v>7015</v>
+      </c>
+      <c r="K93" s="0" t="n">
+        <f aca="false">J93/1000</f>
+        <v>7.015</v>
+      </c>
+      <c r="L93" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>1128</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <f aca="false">D94/1000</f>
+        <v>1.128</v>
+      </c>
+      <c r="F94" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+      <c r="H94" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I94" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J94" s="0" t="n">
+        <v>3012</v>
+      </c>
+      <c r="K94" s="0" t="n">
+        <f aca="false">J94/1000</f>
+        <v>3.012</v>
+      </c>
+      <c r="L94" s="0" t="n">
+        <v>0.999074</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>1408</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <f aca="false">D95/1000</f>
+        <v>1.408</v>
+      </c>
+      <c r="F95" s="0" t="n">
+        <v>0.924704</v>
+      </c>
+      <c r="H95" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I95" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J95" s="0" t="n">
+        <v>3049</v>
+      </c>
+      <c r="K95" s="0" t="n">
+        <f aca="false">J95/1000</f>
+        <v>3.049</v>
+      </c>
+      <c r="L95" s="0" t="n">
+        <v>0.999074</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>5247</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <f aca="false">D96/1000</f>
+        <v>5.247</v>
+      </c>
+      <c r="F96" s="0" t="n">
+        <v>0.976852</v>
+      </c>
+      <c r="H96" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I96" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J96" s="0" t="n">
+        <v>4316</v>
+      </c>
+      <c r="K96" s="0" t="n">
+        <f aca="false">J96/1000</f>
+        <v>4.316</v>
+      </c>
+      <c r="L96" s="0" t="n">
+        <v>0.964815</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>5279</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <f aca="false">D97/1000</f>
+        <v>5.279</v>
+      </c>
+      <c r="F97" s="0" t="n">
+        <v>0.976852</v>
+      </c>
+      <c r="H97" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I97" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J97" s="0" t="n">
+        <v>1339</v>
+      </c>
+      <c r="K97" s="0" t="n">
+        <f aca="false">J97/1000</f>
+        <v>1.339</v>
+      </c>
+      <c r="L97" s="0" t="n">
+        <v>0.976852</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>1534</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <f aca="false">D98/1000</f>
+        <v>1.534</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>0.952778</v>
+      </c>
+      <c r="H98" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I98" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J98" s="0" t="n">
+        <v>1156</v>
+      </c>
+      <c r="K98" s="0" t="n">
+        <f aca="false">J98/1000</f>
+        <v>1.156</v>
+      </c>
+      <c r="L98" s="0" t="n">
+        <v>0.796296</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>1272</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <f aca="false">D99/1000</f>
+        <v>1.272</v>
+      </c>
+      <c r="F99" s="0" t="n">
+        <v>0.974999</v>
+      </c>
+      <c r="H99" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I99" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J99" s="0" t="n">
+        <v>1201</v>
+      </c>
+      <c r="K99" s="0" t="n">
+        <f aca="false">J99/1000</f>
+        <v>1.201</v>
+      </c>
+      <c r="L99" s="0" t="n">
+        <v>0.796296</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="5"/>
+      <c r="H100" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I100" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J100" s="0" t="n">
+        <v>1297</v>
+      </c>
+      <c r="K100" s="0" t="n">
+        <f aca="false">J100/1000</f>
+        <v>1.297</v>
+      </c>
+      <c r="L100" s="0" t="n">
+        <v>0.952778</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="5"/>
+      <c r="H101" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I101" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J101" s="0" t="n">
+        <v>1337</v>
+      </c>
+      <c r="K101" s="0" t="n">
+        <f aca="false">J101/1000</f>
+        <v>1.337</v>
+      </c>
+      <c r="L101" s="0" t="n">
+        <v>0.952778</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E102" s="0" t="n">
+        <f aca="false">AVERAGE(E89:E93)</f>
+        <v>26.305</v>
+      </c>
+      <c r="F102" s="0" t="n">
+        <f aca="false">AVERAGE(F89:F93)</f>
+        <v>1</v>
+      </c>
+      <c r="K102" s="0" t="n">
+        <f aca="false">AVERAGE(K89:K93)</f>
+        <v>5.4416</v>
+      </c>
+      <c r="L102" s="0" t="n">
+        <f aca="false">AVERAGE(L89:L93)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <f aca="false">AVERAGE(E94:E99)</f>
+        <v>2.64466666666667</v>
+      </c>
+      <c r="F103" s="0" t="n">
+        <f aca="false">AVERAGE(F94:F99)</f>
+        <v>0.921401166666667</v>
+      </c>
+      <c r="K103" s="0" t="n">
+        <f aca="false">AVERAGE(K94:K101)</f>
+        <v>2.088375</v>
+      </c>
+      <c r="L103" s="0" t="n">
+        <f aca="false">AVERAGE(L94:L101)</f>
+        <v>0.929745375</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B105" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>4616</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <f aca="false">D105/1000</f>
+        <v>4.616</v>
+      </c>
+      <c r="F105" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H105" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I105" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J105" s="0" t="n">
+        <v>98292</v>
+      </c>
+      <c r="K105" s="0" t="n">
+        <f aca="false">J105/1000</f>
+        <v>98.292</v>
+      </c>
+      <c r="L105" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <v>4064</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <f aca="false">D106/1000</f>
+        <v>4.064</v>
+      </c>
+      <c r="F106" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H106" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I106" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J106" s="0" t="n">
+        <v>44459</v>
+      </c>
+      <c r="K106" s="0" t="n">
+        <f aca="false">J106/1000</f>
+        <v>44.459</v>
+      </c>
+      <c r="L106" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <v>7238</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <f aca="false">D107/1000</f>
+        <v>7.238</v>
+      </c>
+      <c r="F107" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H107" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I107" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J107" s="0" t="n">
+        <v>249848</v>
+      </c>
+      <c r="K107" s="0" t="n">
+        <f aca="false">J107/1000</f>
+        <v>249.848</v>
+      </c>
+      <c r="L107" s="0" t="n">
+        <v>0.076923</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D108" s="0" t="n">
+        <v>4397</v>
+      </c>
+      <c r="E108" s="0" t="n">
+        <f aca="false">D108/1000</f>
+        <v>4.397</v>
+      </c>
+      <c r="F108" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H108" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I108" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J108" s="0" t="n">
+        <v>32025</v>
+      </c>
+      <c r="K108" s="0" t="n">
+        <f aca="false">J108/1000</f>
+        <v>32.025</v>
+      </c>
+      <c r="L108" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <v>3623</v>
+      </c>
+      <c r="E109" s="0" t="n">
+        <f aca="false">D109/1000</f>
+        <v>3.623</v>
+      </c>
+      <c r="F109" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H109" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I109" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J109" s="0" t="n">
+        <v>6950</v>
+      </c>
+      <c r="K109" s="0" t="n">
+        <f aca="false">J109/1000</f>
+        <v>6.95</v>
+      </c>
+      <c r="L109" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <v>3331</v>
+      </c>
+      <c r="E110" s="0" t="n">
+        <f aca="false">D110/1000</f>
+        <v>3.331</v>
+      </c>
+      <c r="F110" s="0" t="n">
+        <v>0.914815</v>
+      </c>
+      <c r="H110" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I110" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J110" s="0" t="n">
+        <v>6176</v>
+      </c>
+      <c r="K110" s="0" t="n">
+        <f aca="false">J110/1000</f>
+        <v>6.176</v>
+      </c>
+      <c r="L110" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D111" s="0" t="n">
+        <v>3382</v>
+      </c>
+      <c r="E111" s="0" t="n">
+        <f aca="false">D111/1000</f>
+        <v>3.382</v>
+      </c>
+      <c r="F111" s="0" t="n">
+        <v>0.914815</v>
+      </c>
+      <c r="H111" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I111" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J111" s="0" t="n">
+        <v>8444</v>
+      </c>
+      <c r="K111" s="0" t="n">
+        <f aca="false">J111/1000</f>
+        <v>8.444</v>
+      </c>
+      <c r="L111" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D112" s="0" t="n">
+        <v>5253</v>
+      </c>
+      <c r="E112" s="0" t="n">
+        <f aca="false">D112/1000</f>
+        <v>5.253</v>
+      </c>
+      <c r="F112" s="0" t="n">
+        <v>0.818518</v>
+      </c>
+      <c r="H112" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I112" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J112" s="0" t="n">
+        <v>5722</v>
+      </c>
+      <c r="K112" s="0" t="n">
+        <f aca="false">J112/1000</f>
+        <v>5.722</v>
+      </c>
+      <c r="L112" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D113" s="0" t="n">
+        <v>1488</v>
+      </c>
+      <c r="E113" s="0" t="n">
+        <f aca="false">D113/1000</f>
+        <v>1.488</v>
+      </c>
+      <c r="F113" s="0" t="n">
+        <v>0.734259</v>
+      </c>
+      <c r="H113" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I113" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J113" s="0" t="n">
+        <v>11487</v>
+      </c>
+      <c r="K113" s="0" t="n">
+        <f aca="false">J113/1000</f>
+        <v>11.487</v>
+      </c>
+      <c r="L113" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <v>2080</v>
+      </c>
+      <c r="E114" s="0" t="n">
+        <f aca="false">D114/1000</f>
+        <v>2.08</v>
+      </c>
+      <c r="F114" s="0" t="n">
+        <v>0.904629</v>
+      </c>
+      <c r="H114" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I114" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J114" s="0" t="n">
+        <v>11519</v>
+      </c>
+      <c r="K114" s="0" t="n">
+        <f aca="false">J114/1000</f>
+        <v>11.519</v>
+      </c>
+      <c r="L114" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <v>2475</v>
+      </c>
+      <c r="E115" s="0" t="n">
+        <f aca="false">D115/1000</f>
+        <v>2.475</v>
+      </c>
+      <c r="F115" s="0" t="n">
+        <v>0.987036</v>
+      </c>
+      <c r="H115" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I115" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J115" s="0" t="n">
+        <v>4755</v>
+      </c>
+      <c r="K115" s="0" t="n">
+        <f aca="false">J115/1000</f>
+        <v>4.755</v>
+      </c>
+      <c r="L115" s="0" t="n">
+        <v>0.5095</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <v>2542</v>
+      </c>
+      <c r="E116" s="0" t="n">
+        <f aca="false">D116/1000</f>
+        <v>2.542</v>
+      </c>
+      <c r="F116" s="0" t="n">
+        <v>0.987036</v>
+      </c>
+      <c r="H116" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I116" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J116" s="0" t="n">
+        <v>21511</v>
+      </c>
+      <c r="K116" s="0" t="n">
+        <f aca="false">J116/1000</f>
+        <v>21.511</v>
+      </c>
+      <c r="L116" s="0" t="n">
+        <v>0.916667</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <v>4828</v>
+      </c>
+      <c r="E117" s="0" t="n">
+        <f aca="false">D117/1000</f>
+        <v>4.828</v>
+      </c>
+      <c r="F117" s="0" t="n">
+        <v>0.89074</v>
+      </c>
+      <c r="H117" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I117" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J117" s="0" t="n">
+        <v>16928</v>
+      </c>
+      <c r="K117" s="0" t="n">
+        <f aca="false">J117/1000</f>
+        <v>16.928</v>
+      </c>
+      <c r="L117" s="0" t="n">
+        <v>0.23071</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <v>3034</v>
+      </c>
+      <c r="E118" s="0" t="n">
+        <f aca="false">D118/1000</f>
+        <v>3.034</v>
+      </c>
+      <c r="F118" s="0" t="n">
+        <v>0.999073</v>
+      </c>
+      <c r="H118" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I118" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J118" s="0" t="n">
+        <v>33655</v>
+      </c>
+      <c r="K118" s="0" t="n">
+        <f aca="false">J118/1000</f>
+        <v>33.655</v>
+      </c>
+      <c r="L118" s="0" t="n">
+        <v>0.999074</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D119" s="0" t="n">
+        <v>2227</v>
+      </c>
+      <c r="E119" s="0" t="n">
+        <f aca="false">D119/1000</f>
+        <v>2.227</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>0.999073</v>
+      </c>
+      <c r="H119" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I119" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J119" s="0" t="n">
+        <v>10807</v>
+      </c>
+      <c r="K119" s="0" t="n">
+        <f aca="false">J119/1000</f>
+        <v>10.807</v>
+      </c>
+      <c r="L119" s="0" t="n">
+        <v>0.571759</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <v>2952</v>
+      </c>
+      <c r="E120" s="0" t="n">
+        <f aca="false">D120/1000</f>
+        <v>2.952</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>0.987037</v>
+      </c>
+      <c r="H120" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I120" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J120" s="0" t="n">
+        <v>888</v>
+      </c>
+      <c r="K120" s="0" t="n">
+        <f aca="false">J120/1000</f>
+        <v>0.888</v>
+      </c>
+      <c r="L120" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D121" s="0" t="n">
+        <v>2426</v>
+      </c>
+      <c r="E121" s="0" t="n">
+        <f aca="false">D121/1000</f>
+        <v>2.426</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>0.166667</v>
+      </c>
+      <c r="H121" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I121" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J121" s="0" t="n">
+        <v>5219</v>
+      </c>
+      <c r="K121" s="0" t="n">
+        <f aca="false">J121/1000</f>
+        <v>5.219</v>
+      </c>
+      <c r="L121" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D122" s="0" t="n">
+        <v>2944</v>
+      </c>
+      <c r="E122" s="0" t="n">
+        <f aca="false">D122/1000</f>
+        <v>2.944</v>
+      </c>
+      <c r="F122" s="0" t="n">
+        <v>0.999073</v>
+      </c>
+      <c r="H122" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I122" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J122" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="K122" s="0" t="n">
+        <f aca="false">J122/1000</f>
+        <v>0.456</v>
+      </c>
+      <c r="L122" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H123" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I123" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J123" s="0" t="n">
+        <v>4642</v>
+      </c>
+      <c r="K123" s="0" t="n">
+        <f aca="false">J123/1000</f>
+        <v>4.642</v>
+      </c>
+      <c r="L123" s="0" t="n">
+        <v>0.976852</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H124" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I124" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J124" s="0" t="n">
+        <v>4044</v>
+      </c>
+      <c r="K124" s="0" t="n">
+        <f aca="false">J124/1000</f>
+        <v>4.044</v>
+      </c>
+      <c r="L124" s="0" t="n">
+        <v>0.9287</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E125" s="0" t="n">
+        <f aca="false">AVERAGE(E105:E109)</f>
+        <v>4.7876</v>
+      </c>
+      <c r="F125" s="0" t="n">
+        <f aca="false">AVERAGE(F105:F109)</f>
+        <v>0.9</v>
+      </c>
+      <c r="K125" s="0" t="n">
+        <f aca="false">AVERAGE(K105:K112)</f>
+        <v>56.4895</v>
+      </c>
+      <c r="L125" s="0" t="n">
+        <f aca="false">AVERAGE(L105:L112)</f>
+        <v>0.717948625</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E126" s="0" t="n">
+        <f aca="false">AVERAGE(E110:E122)</f>
+        <v>2.99707692307692</v>
+      </c>
+      <c r="F126" s="0" t="n">
+        <f aca="false">AVERAGE(F110:F122)</f>
+        <v>0.869443923076923</v>
+      </c>
+      <c r="K126" s="0" t="n">
+        <f aca="false">AVERAGE(K113:K124)</f>
+        <v>10.4925833333333</v>
+      </c>
+      <c r="L126" s="0" t="n">
+        <f aca="false">AVERAGE(L113:L124)</f>
+        <v>0.728697666666667</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B128" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D128" s="0" t="n">
+        <v>30606</v>
+      </c>
+      <c r="E128" s="0" t="n">
+        <f aca="false">D128/1000</f>
+        <v>30.606</v>
+      </c>
+      <c r="F128" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H128" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I128" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J128" s="0" t="n">
+        <v>26061</v>
+      </c>
+      <c r="K128" s="0" t="n">
+        <f aca="false">J128/1000</f>
+        <v>26.061</v>
+      </c>
+      <c r="L128" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B129" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D129" s="0" t="n">
+        <v>50347</v>
+      </c>
+      <c r="E129" s="0" t="n">
+        <f aca="false">D129/1000</f>
+        <v>50.347</v>
+      </c>
+      <c r="F129" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H129" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I129" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J129" s="0" t="n">
+        <v>40399</v>
+      </c>
+      <c r="K129" s="0" t="n">
+        <f aca="false">J129/1000</f>
+        <v>40.399</v>
+      </c>
+      <c r="L129" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B130" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D130" s="0" t="n">
+        <v>24388</v>
+      </c>
+      <c r="E130" s="0" t="n">
+        <f aca="false">D130/1000</f>
+        <v>24.388</v>
+      </c>
+      <c r="F130" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H130" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I130" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J130" s="0" t="n">
+        <v>47868</v>
+      </c>
+      <c r="K130" s="0" t="n">
+        <f aca="false">J130/1000</f>
+        <v>47.868</v>
+      </c>
+      <c r="L130" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B131" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D131" s="0" t="n">
+        <v>26767</v>
+      </c>
+      <c r="E131" s="0" t="n">
+        <f aca="false">D131/1000</f>
+        <v>26.767</v>
+      </c>
+      <c r="F131" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H131" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I131" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J131" s="0" t="n">
+        <v>22067</v>
+      </c>
+      <c r="K131" s="0" t="n">
+        <f aca="false">J131/1000</f>
+        <v>22.067</v>
+      </c>
+      <c r="L131" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B132" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D132" s="0" t="n">
+        <v>118466</v>
+      </c>
+      <c r="E132" s="0" t="n">
+        <f aca="false">D132/1000</f>
+        <v>118.466</v>
+      </c>
+      <c r="F132" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+      <c r="H132" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I132" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J132" s="0" t="n">
+        <v>25233</v>
+      </c>
+      <c r="K132" s="0" t="n">
+        <f aca="false">J132/1000</f>
+        <v>25.233</v>
+      </c>
+      <c r="L132" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B133" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D133" s="0" t="n">
+        <v>120939</v>
+      </c>
+      <c r="E133" s="0" t="n">
+        <f aca="false">D133/1000</f>
+        <v>120.939</v>
+      </c>
+      <c r="F133" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+      <c r="H133" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I133" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J133" s="0" t="n">
+        <v>29519</v>
+      </c>
+      <c r="K133" s="0" t="n">
+        <f aca="false">J133/1000</f>
+        <v>29.519</v>
+      </c>
+      <c r="L133" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B134" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C134" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" s="0" t="n">
+        <v>374</v>
+      </c>
+      <c r="E134" s="0" t="n">
+        <f aca="false">D134/1000</f>
+        <v>0.374</v>
+      </c>
+      <c r="F134" s="0" t="n">
+        <v>0.722222</v>
+      </c>
+      <c r="H134" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I134" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J134" s="0" t="n">
+        <v>30250</v>
+      </c>
+      <c r="K134" s="0" t="n">
+        <f aca="false">J134/1000</f>
+        <v>30.25</v>
+      </c>
+      <c r="L134" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B135" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D135" s="0" t="n">
+        <v>9129</v>
+      </c>
+      <c r="E135" s="0" t="n">
+        <f aca="false">D135/1000</f>
+        <v>9.129</v>
+      </c>
+      <c r="F135" s="0" t="n">
+        <v>0.908796</v>
+      </c>
+      <c r="H135" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I135" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J135" s="0" t="n">
+        <v>33797</v>
+      </c>
+      <c r="K135" s="0" t="n">
+        <f aca="false">J135/1000</f>
+        <v>33.797</v>
+      </c>
+      <c r="L135" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B136" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C136" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136" s="0" t="n">
+        <v>21972</v>
+      </c>
+      <c r="E136" s="0" t="n">
+        <f aca="false">D136/1000</f>
+        <v>21.972</v>
+      </c>
+      <c r="F136" s="0" t="n">
+        <v>0.946759</v>
+      </c>
+      <c r="H136" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I136" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J136" s="0" t="n">
+        <v>47033</v>
+      </c>
+      <c r="K136" s="0" t="n">
+        <f aca="false">J136/1000</f>
+        <v>47.033</v>
+      </c>
+      <c r="L136" s="0" t="n">
+        <v>0.333333</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B137" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D137" s="0" t="n">
+        <v>10319</v>
+      </c>
+      <c r="E137" s="0" t="n">
+        <f aca="false">D137/1000</f>
+        <v>10.319</v>
+      </c>
+      <c r="F137" s="0" t="n">
+        <v>0.866667</v>
+      </c>
+      <c r="H137" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I137" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J137" s="0" t="n">
+        <v>47580</v>
+      </c>
+      <c r="K137" s="0" t="n">
+        <f aca="false">J137/1000</f>
+        <v>47.58</v>
+      </c>
+      <c r="L137" s="0" t="n">
+        <v>0.142857</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C138" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D138" s="0" t="n">
+        <v>8343</v>
+      </c>
+      <c r="E138" s="0" t="n">
+        <f aca="false">D138/1000</f>
+        <v>8.343</v>
+      </c>
+      <c r="F138" s="0" t="n">
+        <v>0.938889</v>
+      </c>
+      <c r="H138" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I138" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J138" s="0" t="n">
+        <v>78499</v>
+      </c>
+      <c r="K138" s="0" t="n">
+        <f aca="false">J138/1000</f>
+        <v>78.499</v>
+      </c>
+      <c r="L138" s="0" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C139" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D139" s="0" t="n">
+        <v>5412</v>
+      </c>
+      <c r="E139" s="0" t="n">
+        <f aca="false">D139/1000</f>
+        <v>5.412</v>
+      </c>
+      <c r="F139" s="0" t="n">
+        <v>0.940741</v>
+      </c>
+      <c r="H139" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I139" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J139" s="0" t="n">
+        <v>86319</v>
+      </c>
+      <c r="K139" s="0" t="n">
+        <f aca="false">J139/1000</f>
+        <v>86.319</v>
+      </c>
+      <c r="L139" s="0" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B140" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D140" s="0" t="n">
+        <v>4520</v>
+      </c>
+      <c r="E140" s="0" t="n">
+        <f aca="false">D140/1000</f>
+        <v>4.52</v>
+      </c>
+      <c r="F140" s="0" t="n">
+        <v>0.950926</v>
+      </c>
+      <c r="H140" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I140" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J140" s="0" t="n">
+        <v>19399</v>
+      </c>
+      <c r="K140" s="0" t="n">
+        <f aca="false">J140/1000</f>
+        <v>19.399</v>
+      </c>
+      <c r="L140" s="0" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H141" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I141" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J141" s="0" t="n">
+        <v>4992</v>
+      </c>
+      <c r="K141" s="0" t="n">
+        <f aca="false">J141/1000</f>
+        <v>4.992</v>
+      </c>
+      <c r="L141" s="0" t="n">
+        <v>0.868519</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H142" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I142" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J142" s="0" t="n">
+        <v>6836</v>
+      </c>
+      <c r="K142" s="0" t="n">
+        <f aca="false">J142/1000</f>
+        <v>6.836</v>
+      </c>
+      <c r="L142" s="0" t="n">
+        <v>0.086111</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H143" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I143" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J143" s="0" t="n">
+        <v>6872</v>
+      </c>
+      <c r="K143" s="0" t="n">
+        <f aca="false">J143/1000</f>
+        <v>6.872</v>
+      </c>
+      <c r="L143" s="0" t="n">
+        <v>0.086111</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H144" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I144" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J144" s="0" t="n">
+        <v>1251</v>
+      </c>
+      <c r="K144" s="0" t="n">
+        <f aca="false">J144/1000</f>
+        <v>1.251</v>
+      </c>
+      <c r="L144" s="0" t="n">
+        <v>0.976852</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H145" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I145" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J145" s="0" t="n">
+        <v>1283</v>
+      </c>
+      <c r="K145" s="0" t="n">
+        <f aca="false">J145/1000</f>
+        <v>1.283</v>
+      </c>
+      <c r="L145" s="0" t="n">
+        <v>0.976852</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H146" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I146" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J146" s="0" t="n">
+        <v>1118</v>
+      </c>
+      <c r="K146" s="0" t="n">
+        <f aca="false">J146/1000</f>
+        <v>1.118</v>
+      </c>
+      <c r="L146" s="0" t="n">
+        <v>0.928704</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H147" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I147" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J147" s="0" t="n">
+        <v>1858</v>
+      </c>
+      <c r="K147" s="0" t="n">
+        <f aca="false">J147/1000</f>
+        <v>1.858</v>
+      </c>
+      <c r="L147" s="0" t="n">
+        <v>0.880556</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E148" s="0" t="n">
+        <f aca="false">AVERAGE(E128:E133)</f>
+        <v>61.9188333333333</v>
+      </c>
+      <c r="F148" s="0" t="n">
+        <f aca="false">AVERAGE(F128:F133)</f>
+        <v>0.569444333333333</v>
+      </c>
+      <c r="K148" s="0" t="n">
+        <f aca="false">AVERAGE(K128:K140)</f>
+        <v>41.0787692307692</v>
+      </c>
+      <c r="L148" s="0" t="n">
+        <f aca="false">AVERAGE(L128:L140)</f>
+        <v>0.445604230769231</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B149" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E149" s="0" t="n">
+        <f aca="false">AVERAGE(E134:E140)</f>
+        <v>8.58128571428572</v>
+      </c>
+      <c r="F149" s="0" t="n">
+        <f aca="false">AVERAGE(F134:F140)</f>
+        <v>0.896428571428571</v>
+      </c>
+      <c r="K149" s="0" t="n">
+        <f aca="false">AVERAGE(K141:K147)</f>
+        <v>3.45857142857143</v>
+      </c>
+      <c r="L149" s="0" t="n">
+        <f aca="false">AVERAGE(L141:L147)</f>
+        <v>0.686243571428571</v>
       </c>
     </row>
   </sheetData>
@@ -3966,27 +5862,27 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9540816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.8214285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3520408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="12.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.515306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4336734693878"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8214285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.515306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.1938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3994,7 +5890,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4002,28 +5898,28 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4175,140 +6071,200 @@
       <c r="A10" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="B10" s="0" t="n">
+        <v>26.305</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2.64466666666667</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.921401166666667</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>5.4416</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>2.088375</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.929745375</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="B11" s="0" t="n">
+        <v>4.7876</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2.99707692307692</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.869443923076923</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>56.4895</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.717948625</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>10.4925833333333</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0.728697666666667</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="B12" s="0" t="n">
+        <v>61.9188333333333</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.569444333333333</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>8.58128571428572</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.896428571428571</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>41.0787692307692</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0.445604230769231</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>3.45857142857143</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0.686243571428571</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B14" s="0" t="n">
         <f aca="false">AVERAGE(B5:B12)</f>
-        <v>7.96619</v>
+        <v>16.6052979166667</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">AVERAGE(C5:C12)</f>
-        <v>0.764733333332</v>
+        <v>0.786638874999167</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">AVERAGE(D5:D12)</f>
-        <v>5.31285428571429</v>
+        <v>5.09841259157509</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">AVERAGE(E5:E12)</f>
-        <v>0.92354406</v>
+        <v>0.91312424514652</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">AVERAGE(F5:F12)</f>
-        <v>95.5007166666667</v>
+        <v>72.5641815705128</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">AVERAGE(G5:G12)</f>
-        <v>0.661249936111111</v>
+        <v>0.683725317040598</v>
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">AVERAGE(H5:H12)</f>
-        <v>14.9229297619048</v>
+        <v>11.3317723214286</v>
       </c>
       <c r="I14" s="0" t="n">
         <f aca="false">AVERAGE(I5:I12)</f>
-        <v>0.814976026190476</v>
+        <v>0.802445843005952</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B15" s="0" t="n">
-        <f aca="false">STDEV(B5:B9)</f>
-        <v>2.93033301656996</v>
+        <f aca="false">STDEV(B5:B12)</f>
+        <v>19.6198770596249</v>
       </c>
       <c r="C15" s="0" t="n">
-        <f aca="false">STDEV(C5:C9)</f>
-        <v>0.245988527283386</v>
+        <f aca="false">STDEV(C5:C12)</f>
+        <v>0.223602922690892</v>
       </c>
       <c r="D15" s="0" t="n">
-        <f aca="false">STDEV(D5:D9)</f>
-        <v>0.663615294444309</v>
+        <f aca="false">STDEV(D5:D12)</f>
+        <v>1.87305529937493</v>
       </c>
       <c r="E15" s="0" t="n">
-        <f aca="false">STDEV(E5:E9)</f>
-        <v>0.0564145791473091</v>
+        <f aca="false">STDEV(E5:E12)</f>
+        <v>0.0470994467001571</v>
       </c>
       <c r="F15" s="0" t="n">
-        <f aca="false">STDEV(F5:F9)</f>
-        <v>90.9401425299782</v>
+        <f aca="false">STDEV(F5:F12)</f>
+        <v>76.9656962911434</v>
       </c>
       <c r="G15" s="0" t="n">
-        <f aca="false">STDEV(G5:G9)</f>
-        <v>0.319341981926465</v>
+        <f aca="false">STDEV(G5:G12)</f>
+        <v>0.284942470644346</v>
       </c>
       <c r="H15" s="0" t="n">
-        <f aca="false">STDEV(H5:H9)</f>
-        <v>11.1627239238309</v>
+        <f aca="false">STDEV(H5:H12)</f>
+        <v>10.0785458482641</v>
       </c>
       <c r="I15" s="0" t="n">
-        <f aca="false">STDEV(I5:I9)</f>
-        <v>0.097881374897099</v>
+        <f aca="false">STDEV(I5:I12)</f>
+        <v>0.102994461667462</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>7.96619</v>
+        <v>16.6052979166667</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>95.5007166666667</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>2.93033301656996</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>90.9401425299782</v>
+        <v>72.5641815705128</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>5.31285428571429</v>
+        <v>5.09841259157509</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>14.9229297619048</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>0.663615294444309</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>11.1627239238309</v>
+        <v>11.3317723214286</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4316,41 +6272,29 @@
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>0.764733333332</v>
+        <v>0.786638874999167</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>0.661249936111111</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>0.245988527283386</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>0.319341981926465</v>
+        <v>0.683725317040598</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.92354406</v>
+        <v>0.91312424514652</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>0.814976026190476</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>0.0564145791473091</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>0.097881374897099</v>
+        <v>0.802445843005952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>